<commit_message>
Exceltabelle erweitert; Automatisch Endzeitdatum füllen falls NULL war
</commit_message>
<xml_diff>
--- a/PythonCode/mysite/Personen.xlsx
+++ b/PythonCode/mysite/Personen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephan/Desktop/Waldorf Lockin Projekt/PythonCode/mysite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEE53CE-3E5F-7548-BF03-216C040CB0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6F4825-879B-0C41-A6A1-ED9ACFA7D8B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="4580" windowWidth="27840" windowHeight="16740" xr2:uid="{A1001FAB-5DBF-5B43-A8B0-67389FE9DBAD}"/>
+    <workbookView xWindow="5680" yWindow="4160" windowWidth="27840" windowHeight="16740" xr2:uid="{A1001FAB-5DBF-5B43-A8B0-67389FE9DBAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Klasse</t>
   </si>
@@ -56,18 +56,12 @@
     <t>Mustermann</t>
   </si>
   <si>
-    <t>10x</t>
-  </si>
-  <si>
     <t>Stephan</t>
   </si>
   <si>
     <t>Fuchs</t>
   </si>
   <si>
-    <t>3C</t>
-  </si>
-  <si>
     <t>Max</t>
   </si>
   <si>
@@ -87,6 +81,30 @@
   </si>
   <si>
     <t>1a</t>
+  </si>
+  <si>
+    <t>Emmy</t>
+  </si>
+  <si>
+    <t>Watson</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>Johanna</t>
+  </si>
+  <si>
+    <t>Orlean</t>
+  </si>
+  <si>
+    <t>2b</t>
+  </si>
+  <si>
+    <t>3b</t>
+  </si>
+  <si>
+    <t>10a</t>
   </si>
 </sst>
 </file>
@@ -168,9 +186,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +226,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -314,7 +332,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -456,7 +474,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -464,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90347F0-82B4-7340-AD1B-F67758E68567}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,10 +495,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -505,26 +523,26 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -532,13 +550,35 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
         <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>